<commit_message>
removed rtools so it will push to GitHub
</commit_message>
<xml_diff>
--- a/actual_data.xlsx
+++ b/actual_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michigantech-my.sharepoint.com/personal/tmbarnes_mtu_edu/Documents/PhD/Chapter1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="552" documentId="8_{3D855F46-538B-4866-82C0-B62F336DDD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AFFF55C-43AA-4A1F-8975-15498991DC59}"/>
+  <xr:revisionPtr revIDLastSave="598" documentId="8_{3D855F46-538B-4866-82C0-B62F336DDD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B479F1C8-2F16-4A38-8D15-9430519095C8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3550" yWindow="600" windowWidth="14400" windowHeight="7270" xr2:uid="{F0AB33CE-9D66-4394-A1B2-6EBAD4716641}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{F0AB33CE-9D66-4394-A1B2-6EBAD4716641}"/>
   </bookViews>
   <sheets>
     <sheet name="actual_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="38">
   <si>
     <t>site</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Mass  C Adit</t>
+  </si>
+  <si>
+    <t>Keel Ridge Mine</t>
   </si>
 </sst>
 </file>
@@ -627,12 +630,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1012,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1A3417-2E4A-4A3D-A021-85D92EBEF949}">
-  <dimension ref="A1:M196"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="E198" sqref="E198"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1027,6 +1031,7 @@
     <col min="10" max="10" width="10.81640625" customWidth="1"/>
     <col min="11" max="11" width="11.453125" customWidth="1"/>
     <col min="13" max="13" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -6205,7 +6210,7 @@
         <v>19</v>
       </c>
       <c r="G153">
-        <f t="shared" ref="G153:G196" si="6">(F153-I153)/(J153-I153)</f>
+        <f t="shared" ref="G153:G213" si="6">(F153-I153)/(J153-I153)</f>
         <v>0</v>
       </c>
       <c r="H153">
@@ -7601,7 +7606,7 @@
         <v>4.2592592592592604</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>36</v>
       </c>
@@ -7637,7 +7642,7 @@
         <v>4.2592592592592604</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>36</v>
       </c>
@@ -7673,7 +7678,7 @@
         <v>4.2592592592592604</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>36</v>
       </c>
@@ -7709,7 +7714,7 @@
         <v>4.2592592592592604</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>36</v>
       </c>
@@ -7743,6 +7748,633 @@
       </c>
       <c r="M196">
         <v>4.2592592592592604</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>37</v>
+      </c>
+      <c r="D197">
+        <v>1996</v>
+      </c>
+      <c r="F197">
+        <v>242</v>
+      </c>
+      <c r="G197">
+        <f t="shared" si="6"/>
+        <v>0.79762611275964401</v>
+      </c>
+      <c r="H197">
+        <v>1996</v>
+      </c>
+      <c r="I197">
+        <v>18</v>
+      </c>
+      <c r="J197">
+        <v>298.83333333333331</v>
+      </c>
+      <c r="K197">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L197">
+        <v>2024</v>
+      </c>
+      <c r="M197">
+        <v>7.2222222222222197</v>
+      </c>
+      <c r="N197" s="3">
+        <v>35069</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>37</v>
+      </c>
+      <c r="D198">
+        <v>2004</v>
+      </c>
+      <c r="F198">
+        <v>393</v>
+      </c>
+      <c r="G198">
+        <f t="shared" si="6"/>
+        <v>1.3353115727002969</v>
+      </c>
+      <c r="H198">
+        <v>2005</v>
+      </c>
+      <c r="I198">
+        <v>18</v>
+      </c>
+      <c r="J198">
+        <v>298.83333333333331</v>
+      </c>
+      <c r="K198">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L198">
+        <v>2024</v>
+      </c>
+      <c r="M198">
+        <v>8.8888888888888893</v>
+      </c>
+      <c r="N198" s="3">
+        <v>38350</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>37</v>
+      </c>
+      <c r="D199">
+        <v>2007</v>
+      </c>
+      <c r="F199">
+        <v>267</v>
+      </c>
+      <c r="G199">
+        <f t="shared" si="6"/>
+        <v>0.8866468842729982</v>
+      </c>
+      <c r="H199">
+        <v>2007</v>
+      </c>
+      <c r="I199">
+        <v>18</v>
+      </c>
+      <c r="J199">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K199">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L199">
+        <v>2024</v>
+      </c>
+      <c r="M199">
+        <v>7.5</v>
+      </c>
+      <c r="N199" s="3">
+        <v>39165</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>37</v>
+      </c>
+      <c r="D200">
+        <v>2009</v>
+      </c>
+      <c r="F200">
+        <v>203</v>
+      </c>
+      <c r="G200">
+        <f t="shared" si="6"/>
+        <v>0.65875370919881393</v>
+      </c>
+      <c r="H200">
+        <v>2009</v>
+      </c>
+      <c r="I200">
+        <v>18</v>
+      </c>
+      <c r="J200">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K200">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L200">
+        <v>2024</v>
+      </c>
+      <c r="M200">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N200" s="3">
+        <v>39893</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>37</v>
+      </c>
+      <c r="D201">
+        <v>2009</v>
+      </c>
+      <c r="F201">
+        <v>275</v>
+      </c>
+      <c r="G201">
+        <f t="shared" si="6"/>
+        <v>0.91513353115727125</v>
+      </c>
+      <c r="H201">
+        <v>2010</v>
+      </c>
+      <c r="I201">
+        <v>18</v>
+      </c>
+      <c r="J201">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K201">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L201">
+        <v>2024</v>
+      </c>
+      <c r="M201">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N201" s="3">
+        <v>40131</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>37</v>
+      </c>
+      <c r="D202">
+        <v>2010</v>
+      </c>
+      <c r="F202">
+        <v>290</v>
+      </c>
+      <c r="G202">
+        <f t="shared" si="6"/>
+        <v>0.96854599406528319</v>
+      </c>
+      <c r="H202">
+        <v>2010</v>
+      </c>
+      <c r="I202">
+        <v>18</v>
+      </c>
+      <c r="J202">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K202">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L202">
+        <v>2024</v>
+      </c>
+      <c r="M202">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N202" s="3">
+        <v>40264</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>37</v>
+      </c>
+      <c r="D203">
+        <v>2010</v>
+      </c>
+      <c r="F203">
+        <v>324</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="6"/>
+        <v>1.0896142433234435</v>
+      </c>
+      <c r="H203">
+        <v>2011</v>
+      </c>
+      <c r="I203">
+        <v>18</v>
+      </c>
+      <c r="J203">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K203">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L203">
+        <v>2024</v>
+      </c>
+      <c r="M203">
+        <v>9</v>
+      </c>
+      <c r="N203" s="3">
+        <v>40488</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>37</v>
+      </c>
+      <c r="D204">
+        <v>2011</v>
+      </c>
+      <c r="F204">
+        <v>262</v>
+      </c>
+      <c r="G204">
+        <f t="shared" si="6"/>
+        <v>0.86884272997032752</v>
+      </c>
+      <c r="H204">
+        <v>2011</v>
+      </c>
+      <c r="I204">
+        <v>18</v>
+      </c>
+      <c r="J204">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K204">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L204">
+        <v>2024</v>
+      </c>
+      <c r="M204">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N204" s="3">
+        <v>40628</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>37</v>
+      </c>
+      <c r="D205">
+        <v>2013</v>
+      </c>
+      <c r="F205">
+        <v>222</v>
+      </c>
+      <c r="G205">
+        <f t="shared" si="6"/>
+        <v>0.72640949554896239</v>
+      </c>
+      <c r="H205">
+        <v>2013</v>
+      </c>
+      <c r="I205">
+        <v>18</v>
+      </c>
+      <c r="J205">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K205">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L205">
+        <v>2024</v>
+      </c>
+      <c r="M205">
+        <v>8.6388888888888893</v>
+      </c>
+      <c r="N205" s="3">
+        <v>41348</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>37</v>
+      </c>
+      <c r="D206">
+        <v>2014</v>
+      </c>
+      <c r="F206">
+        <v>300</v>
+      </c>
+      <c r="G206">
+        <f t="shared" si="6"/>
+        <v>1.0041543026706243</v>
+      </c>
+      <c r="H206">
+        <v>2014</v>
+      </c>
+      <c r="I206">
+        <v>18</v>
+      </c>
+      <c r="J206">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K206">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L206">
+        <v>2024</v>
+      </c>
+      <c r="M206">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N206" s="3">
+        <v>41694</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>37</v>
+      </c>
+      <c r="D207">
+        <v>2015</v>
+      </c>
+      <c r="F207">
+        <v>587</v>
+      </c>
+      <c r="G207">
+        <f t="shared" si="6"/>
+        <v>2.0261127596439197</v>
+      </c>
+      <c r="H207">
+        <v>2015</v>
+      </c>
+      <c r="I207">
+        <v>18</v>
+      </c>
+      <c r="J207">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K207">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L207">
+        <v>2024</v>
+      </c>
+      <c r="M207">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N207" s="3">
+        <v>42057</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>37</v>
+      </c>
+      <c r="D208">
+        <v>2016</v>
+      </c>
+      <c r="F208">
+        <v>221</v>
+      </c>
+      <c r="G208">
+        <f t="shared" si="6"/>
+        <v>0.72284866468842823</v>
+      </c>
+      <c r="H208">
+        <v>2016</v>
+      </c>
+      <c r="I208">
+        <v>18</v>
+      </c>
+      <c r="J208">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K208">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L208">
+        <v>2024</v>
+      </c>
+      <c r="M208">
+        <v>8.0555555555555607</v>
+      </c>
+      <c r="N208" s="3">
+        <v>42420</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>37</v>
+      </c>
+      <c r="D209">
+        <v>2017</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>45</v>
+      </c>
+      <c r="G209">
+        <f t="shared" si="6"/>
+        <v>9.6142433234421482E-2</v>
+      </c>
+      <c r="H209">
+        <v>2017</v>
+      </c>
+      <c r="I209">
+        <v>18</v>
+      </c>
+      <c r="J209">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K209">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L209">
+        <v>2024</v>
+      </c>
+      <c r="M209">
+        <v>8.25</v>
+      </c>
+      <c r="N209" s="3">
+        <v>42777</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>37</v>
+      </c>
+      <c r="D210">
+        <v>2019</v>
+      </c>
+      <c r="E210">
+        <v>2</v>
+      </c>
+      <c r="F210">
+        <v>103</v>
+      </c>
+      <c r="G210">
+        <f t="shared" si="6"/>
+        <v>0.302670623145401</v>
+      </c>
+      <c r="H210">
+        <v>2019</v>
+      </c>
+      <c r="I210">
+        <v>18</v>
+      </c>
+      <c r="J210">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K210">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L210">
+        <v>2024</v>
+      </c>
+      <c r="M210">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N210" s="3">
+        <v>43479</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>37</v>
+      </c>
+      <c r="D211">
+        <v>2021</v>
+      </c>
+      <c r="E211">
+        <v>4</v>
+      </c>
+      <c r="F211">
+        <v>107</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="6"/>
+        <v>0.31691394658753752</v>
+      </c>
+      <c r="H211">
+        <v>2021</v>
+      </c>
+      <c r="I211">
+        <v>18</v>
+      </c>
+      <c r="J211">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K211">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L211">
+        <v>2024</v>
+      </c>
+      <c r="M211">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N211" s="3">
+        <v>44258</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>37</v>
+      </c>
+      <c r="D212">
+        <v>2023</v>
+      </c>
+      <c r="E212">
+        <v>6</v>
+      </c>
+      <c r="F212">
+        <v>30</v>
+      </c>
+      <c r="G212">
+        <f t="shared" si="6"/>
+        <v>4.2729970326409551E-2</v>
+      </c>
+      <c r="H212">
+        <v>2023</v>
+      </c>
+      <c r="I212">
+        <v>18</v>
+      </c>
+      <c r="J212">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K212">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L212">
+        <v>2024</v>
+      </c>
+      <c r="M212">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="N212" s="3">
+        <v>45028</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>37</v>
+      </c>
+      <c r="D213">
+        <v>2024</v>
+      </c>
+      <c r="E213">
+        <v>7</v>
+      </c>
+      <c r="F213">
+        <v>18</v>
+      </c>
+      <c r="G213">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>2024</v>
+      </c>
+      <c r="I213">
+        <v>18</v>
+      </c>
+      <c r="J213">
+        <v>298.83333333333297</v>
+      </c>
+      <c r="K213">
+        <v>7.9756944444444402</v>
+      </c>
+      <c r="L213">
+        <v>2024</v>
+      </c>
+      <c r="M213">
+        <v>6.25</v>
+      </c>
+      <c r="N213" s="3">
+        <v>45394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>